<commit_message>
Added NN + extension
</commit_message>
<xml_diff>
--- a/mse_434_paper_data.xlsx
+++ b/mse_434_paper_data.xlsx
@@ -1,29 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10720"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dhruvsharma/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dhruvsharma/MSE434/Group_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E981B8-3160-DA48-8649-7946AEF58F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59AD5264-D036-ED46-A3EA-DF05E3E1899F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="30240" windowHeight="19640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17580" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="raw_data" sheetId="1" r:id="rId1"/>
     <sheet name="customers" sheetId="2" r:id="rId2"/>
-    <sheet name="valid_routes" sheetId="3" r:id="rId3"/>
-    <sheet name="customer_routes" sheetId="4" r:id="rId4"/>
+    <sheet name="customers_stress" sheetId="5" r:id="rId3"/>
+    <sheet name="customers_nonstress" sheetId="6" r:id="rId4"/>
+    <sheet name="valid_routes" sheetId="3" r:id="rId5"/>
+    <sheet name="customer_routes" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="36">
   <si>
     <t>Plant</t>
   </si>
@@ -128,13 +130,16 @@
   </si>
   <si>
     <t>[2, 7]</t>
+  </si>
+  <si>
+    <t>—</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -169,6 +174,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -184,7 +204,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -220,11 +240,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -242,6 +277,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,7 +500,9 @@
   </sheetPr>
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -487,7 +527,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -500,7 +540,7 @@
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -517,7 +557,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -534,7 +574,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -551,7 +591,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -568,7 +608,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -585,7 +625,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -602,7 +642,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>7</v>
       </c>
@@ -619,7 +659,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -636,7 +676,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -653,7 +693,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -670,7 +710,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -687,7 +727,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -704,7 +744,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -721,7 +761,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -738,7 +778,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -755,7 +795,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>16</v>
       </c>
@@ -772,7 +812,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>17</v>
       </c>
@@ -789,7 +829,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>18</v>
       </c>
@@ -806,7 +846,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -823,7 +863,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
         <v>20</v>
       </c>
@@ -840,7 +880,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>21</v>
       </c>
@@ -857,7 +897,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>22</v>
       </c>
@@ -874,7 +914,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
         <v>23</v>
       </c>
@@ -891,7 +931,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>24</v>
       </c>
@@ -908,7 +948,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>25</v>
       </c>
@@ -925,7 +965,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>26</v>
       </c>
@@ -942,7 +982,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>27</v>
       </c>
@@ -959,7 +999,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>28</v>
       </c>
@@ -976,7 +1016,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>29</v>
       </c>
@@ -993,7 +1033,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>30</v>
       </c>
@@ -1022,7 +1062,9 @@
   </sheetPr>
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -1046,7 +1088,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -1059,7 +1101,7 @@
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1076,7 +1118,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>7</v>
       </c>
@@ -1093,7 +1135,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>16</v>
       </c>
@@ -1110,7 +1152,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>20</v>
       </c>
@@ -1127,7 +1169,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>23</v>
       </c>
@@ -1150,14 +1192,464 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2420607-5E3A-9444-9712-53DBDC965EE1}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView zoomScale="134" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="7"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="8">
+        <v>17</v>
+      </c>
+      <c r="C2" s="8">
+        <v>52</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A3" s="8">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8">
+        <v>10</v>
+      </c>
+      <c r="C3" s="8">
+        <v>60</v>
+      </c>
+      <c r="D3" s="8">
+        <v>6</v>
+      </c>
+      <c r="E3" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A4" s="8">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8">
+        <v>11.5</v>
+      </c>
+      <c r="C4" s="8">
+        <v>58</v>
+      </c>
+      <c r="D4" s="8">
+        <v>6</v>
+      </c>
+      <c r="E4" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A5" s="8">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8">
+        <v>18</v>
+      </c>
+      <c r="C5" s="8">
+        <v>47</v>
+      </c>
+      <c r="D5" s="8">
+        <v>12</v>
+      </c>
+      <c r="E5" s="8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A6" s="8">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8">
+        <v>20</v>
+      </c>
+      <c r="C6" s="8">
+        <v>45</v>
+      </c>
+      <c r="D6" s="8">
+        <v>19</v>
+      </c>
+      <c r="E6" s="8">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A7" s="8">
+        <v>8</v>
+      </c>
+      <c r="B7" s="8">
+        <v>28</v>
+      </c>
+      <c r="C7" s="8">
+        <v>47.5</v>
+      </c>
+      <c r="D7" s="8">
+        <v>25</v>
+      </c>
+      <c r="E7" s="8">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A8" s="8">
+        <v>10</v>
+      </c>
+      <c r="B8" s="8">
+        <v>30</v>
+      </c>
+      <c r="C8" s="8">
+        <v>50</v>
+      </c>
+      <c r="D8" s="8">
+        <v>20</v>
+      </c>
+      <c r="E8" s="8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A9" s="8">
+        <v>12</v>
+      </c>
+      <c r="B9" s="8">
+        <v>12</v>
+      </c>
+      <c r="C9" s="8">
+        <v>57</v>
+      </c>
+      <c r="D9" s="8">
+        <v>17</v>
+      </c>
+      <c r="E9" s="8">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A10" s="8">
+        <v>13</v>
+      </c>
+      <c r="B10" s="8">
+        <v>26</v>
+      </c>
+      <c r="C10" s="8">
+        <v>49</v>
+      </c>
+      <c r="D10" s="8">
+        <v>12</v>
+      </c>
+      <c r="E10" s="8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A11" s="8">
+        <v>20</v>
+      </c>
+      <c r="B11" s="8">
+        <v>17</v>
+      </c>
+      <c r="C11" s="8">
+        <v>55</v>
+      </c>
+      <c r="D11" s="8">
+        <v>7</v>
+      </c>
+      <c r="E11" s="8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A12" s="8">
+        <v>28</v>
+      </c>
+      <c r="B12" s="8">
+        <v>29</v>
+      </c>
+      <c r="C12" s="8">
+        <v>46</v>
+      </c>
+      <c r="D12" s="8">
+        <v>7</v>
+      </c>
+      <c r="E12" s="8">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F23D0A80-5CD4-1941-9FE6-65CA1DE2B111}">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="8">
+        <v>17</v>
+      </c>
+      <c r="C2" s="8">
+        <v>52</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A3" s="8">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8">
+        <v>17</v>
+      </c>
+      <c r="C3" s="8">
+        <v>54.44</v>
+      </c>
+      <c r="D3" s="8">
+        <v>6</v>
+      </c>
+      <c r="E3" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A4" s="8">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8">
+        <v>15.06</v>
+      </c>
+      <c r="C4" s="8">
+        <v>53.5</v>
+      </c>
+      <c r="D4" s="8">
+        <v>6</v>
+      </c>
+      <c r="E4" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A5" s="8">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8">
+        <v>20.52</v>
+      </c>
+      <c r="C5" s="8">
+        <v>50.34</v>
+      </c>
+      <c r="D5" s="8">
+        <v>12</v>
+      </c>
+      <c r="E5" s="8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A6" s="8">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8">
+        <v>21.77</v>
+      </c>
+      <c r="C6" s="8">
+        <v>50.24</v>
+      </c>
+      <c r="D6" s="8">
+        <v>19</v>
+      </c>
+      <c r="E6" s="8">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A7" s="8">
+        <v>8</v>
+      </c>
+      <c r="B7" s="8">
+        <v>22.22</v>
+      </c>
+      <c r="C7" s="8">
+        <v>50.92</v>
+      </c>
+      <c r="D7" s="8">
+        <v>25</v>
+      </c>
+      <c r="E7" s="8">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A8" s="8">
+        <v>10</v>
+      </c>
+      <c r="B8" s="8">
+        <v>22.82</v>
+      </c>
+      <c r="C8" s="8">
+        <v>52.3</v>
+      </c>
+      <c r="D8" s="8">
+        <v>20</v>
+      </c>
+      <c r="E8" s="8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A9" s="8">
+        <v>12</v>
+      </c>
+      <c r="B9" s="8">
+        <v>15.49</v>
+      </c>
+      <c r="C9" s="8">
+        <v>53.36</v>
+      </c>
+      <c r="D9" s="8">
+        <v>17</v>
+      </c>
+      <c r="E9" s="8">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A10" s="8">
+        <v>13</v>
+      </c>
+      <c r="B10" s="8">
+        <v>22.38</v>
+      </c>
+      <c r="C10" s="8">
+        <v>51.93</v>
+      </c>
+      <c r="D10" s="8">
+        <v>12</v>
+      </c>
+      <c r="E10" s="8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A11" s="8">
+        <v>20</v>
+      </c>
+      <c r="B11" s="8">
+        <v>20.010000000000002</v>
+      </c>
+      <c r="C11" s="8">
+        <v>53.27</v>
+      </c>
+      <c r="D11" s="8">
+        <v>7</v>
+      </c>
+      <c r="E11" s="8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A12" s="8">
+        <v>28</v>
+      </c>
+      <c r="B12" s="8">
+        <v>22.23</v>
+      </c>
+      <c r="C12" s="8">
+        <v>50.07</v>
+      </c>
+      <c r="D12" s="8">
+        <v>7</v>
+      </c>
+      <c r="E12" s="8">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1285,7 +1777,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -1567,7 +2059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated values and corrected Routes
</commit_message>
<xml_diff>
--- a/mse_434_paper_data.xlsx
+++ b/mse_434_paper_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dhruvsharma/MSE434/Group_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59AD5264-D036-ED46-A3EA-DF05E3E1899F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD5C5B45-CEAE-D148-B37D-7C9DE8C8F5D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17580" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17580" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="raw_data" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="100">
   <si>
     <t>Plant</t>
   </si>
@@ -54,92 +54,284 @@
     <t>R1</t>
   </si>
   <si>
-    <t>[2]</t>
-  </si>
-  <si>
     <t>R2</t>
   </si>
   <si>
-    <t>[20]</t>
-  </si>
-  <si>
     <t>R3</t>
   </si>
   <si>
-    <t>[23]</t>
-  </si>
-  <si>
     <t>R4</t>
   </si>
   <si>
-    <t>[16]</t>
-  </si>
-  <si>
     <t>R5</t>
   </si>
   <si>
     <t>R6</t>
   </si>
   <si>
-    <t>[2, 20]</t>
-  </si>
-  <si>
     <t>R7</t>
   </si>
   <si>
-    <t>[2, 23]</t>
-  </si>
-  <si>
     <t>R8</t>
   </si>
   <si>
-    <t>[2, 16]</t>
-  </si>
-  <si>
     <t>R9</t>
   </si>
   <si>
     <t>R10</t>
   </si>
   <si>
-    <t>[20, 23]</t>
-  </si>
-  <si>
     <t>R11</t>
   </si>
   <si>
-    <t>[20, 16]</t>
-  </si>
-  <si>
     <t>R12</t>
   </si>
   <si>
-    <t>[23, 16]</t>
-  </si>
-  <si>
     <t>R13</t>
   </si>
   <si>
-    <t>[2, 20, 23]</t>
-  </si>
-  <si>
     <t>Customer</t>
   </si>
   <si>
-    <t>[7]</t>
-  </si>
-  <si>
-    <t>[2, 7]</t>
-  </si>
-  <si>
     <t>—</t>
+  </si>
+  <si>
+    <t>['2']</t>
+  </si>
+  <si>
+    <t>['3']</t>
+  </si>
+  <si>
+    <t>['4']</t>
+  </si>
+  <si>
+    <t>['5']</t>
+  </si>
+  <si>
+    <t>['8']</t>
+  </si>
+  <si>
+    <t>['10']</t>
+  </si>
+  <si>
+    <t>['12']</t>
+  </si>
+  <si>
+    <t>['13']</t>
+  </si>
+  <si>
+    <t>['20']</t>
+  </si>
+  <si>
+    <t>['28']</t>
+  </si>
+  <si>
+    <t>['2', '3']</t>
+  </si>
+  <si>
+    <t>['2', '4']</t>
+  </si>
+  <si>
+    <t>['2', '5']</t>
+  </si>
+  <si>
+    <t>R14</t>
+  </si>
+  <si>
+    <t>['2', '12']</t>
+  </si>
+  <si>
+    <t>R15</t>
+  </si>
+  <si>
+    <t>['2', '13']</t>
+  </si>
+  <si>
+    <t>R16</t>
+  </si>
+  <si>
+    <t>['2', '20']</t>
+  </si>
+  <si>
+    <t>R17</t>
+  </si>
+  <si>
+    <t>['2', '28']</t>
+  </si>
+  <si>
+    <t>R18</t>
+  </si>
+  <si>
+    <t>['3', '4']</t>
+  </si>
+  <si>
+    <t>R19</t>
+  </si>
+  <si>
+    <t>['3', '5']</t>
+  </si>
+  <si>
+    <t>R20</t>
+  </si>
+  <si>
+    <t>['3', '12']</t>
+  </si>
+  <si>
+    <t>R21</t>
+  </si>
+  <si>
+    <t>['3', '13']</t>
+  </si>
+  <si>
+    <t>R22</t>
+  </si>
+  <si>
+    <t>['3', '20']</t>
+  </si>
+  <si>
+    <t>R23</t>
+  </si>
+  <si>
+    <t>['3', '28']</t>
+  </si>
+  <si>
+    <t>R24</t>
+  </si>
+  <si>
+    <t>['4', '13']</t>
+  </si>
+  <si>
+    <t>R25</t>
+  </si>
+  <si>
+    <t>['4', '20']</t>
+  </si>
+  <si>
+    <t>R26</t>
+  </si>
+  <si>
+    <t>['4', '28']</t>
+  </si>
+  <si>
+    <t>R27</t>
+  </si>
+  <si>
+    <t>['12', '20']</t>
+  </si>
+  <si>
+    <t>R28</t>
+  </si>
+  <si>
+    <t>['12', '28']</t>
+  </si>
+  <si>
+    <t>R29</t>
+  </si>
+  <si>
+    <t>['13', '20']</t>
+  </si>
+  <si>
+    <t>R30</t>
+  </si>
+  <si>
+    <t>['13', '28']</t>
+  </si>
+  <si>
+    <t>R31</t>
+  </si>
+  <si>
+    <t>['20', '28']</t>
+  </si>
+  <si>
+    <t>R32</t>
+  </si>
+  <si>
+    <t>['2', '3', '4']</t>
+  </si>
+  <si>
+    <t>R33</t>
+  </si>
+  <si>
+    <t>['2', '3', '13']</t>
+  </si>
+  <si>
+    <t>R34</t>
+  </si>
+  <si>
+    <t>['2', '3', '20']</t>
+  </si>
+  <si>
+    <t>R35</t>
+  </si>
+  <si>
+    <t>['2', '3', '28']</t>
+  </si>
+  <si>
+    <t>R36</t>
+  </si>
+  <si>
+    <t>['2', '4', '20']</t>
+  </si>
+  <si>
+    <t>R37</t>
+  </si>
+  <si>
+    <t>['2', '4', '28']</t>
+  </si>
+  <si>
+    <t>R38</t>
+  </si>
+  <si>
+    <t>['2', '13', '20']</t>
+  </si>
+  <si>
+    <t>R39</t>
+  </si>
+  <si>
+    <t>['2', '13', '28']</t>
+  </si>
+  <si>
+    <t>R40</t>
+  </si>
+  <si>
+    <t>['2', '20', '28']</t>
+  </si>
+  <si>
+    <t>R41</t>
+  </si>
+  <si>
+    <t>['3', '4', '20']</t>
+  </si>
+  <si>
+    <t>R42</t>
+  </si>
+  <si>
+    <t>['3', '4', '28']</t>
+  </si>
+  <si>
+    <t>R43</t>
+  </si>
+  <si>
+    <t>['3', '13', '20']</t>
+  </si>
+  <si>
+    <t>R44</t>
+  </si>
+  <si>
+    <t>['3', '13', '28']</t>
+  </si>
+  <si>
+    <t>R45</t>
+  </si>
+  <si>
+    <t>['3', '20', '28']</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -189,8 +381,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -201,6 +406,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFF2CC"/>
         <bgColor rgb="FFFFF2CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -259,7 +470,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -280,6 +491,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -501,7 +720,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E32"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -575,54 +794,54 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
+      <c r="A5" s="10">
         <v>3</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="10">
         <v>15.06</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="10">
         <v>53.5</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="10">
         <v>6</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="10">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
+      <c r="A6" s="10">
         <v>4</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="10">
         <v>20.52</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="10">
         <v>50.34</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="10">
         <v>12</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="10">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
+      <c r="A7" s="10">
         <v>5</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="10">
         <v>21.77</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="10">
         <v>50.24</v>
       </c>
-      <c r="D7" s="3">
-        <v>25</v>
-      </c>
-      <c r="E7" s="3">
-        <v>25</v>
+      <c r="D7" s="10">
+        <v>19</v>
+      </c>
+      <c r="E7" s="10">
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.2">
@@ -643,36 +862,36 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A9" s="4">
+      <c r="A9" s="11">
         <v>7</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="11">
         <v>16.96</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="11">
         <v>51.66</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="11">
         <v>18</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="11">
         <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
+      <c r="A10" s="10">
         <v>8</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="10">
         <v>22.22</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="10">
         <v>50.92</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="10">
         <v>25</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="10">
         <v>25</v>
       </c>
     </row>
@@ -694,19 +913,19 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
+      <c r="A12" s="10">
         <v>10</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="10">
         <v>22.82</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="10">
         <v>52.3</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="10">
         <v>20</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="10">
         <v>20</v>
       </c>
     </row>
@@ -728,36 +947,36 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
+      <c r="A14" s="10">
         <v>12</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="10">
         <v>15.49</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="10">
         <v>53.36</v>
       </c>
-      <c r="D14" s="3">
-        <v>24</v>
-      </c>
-      <c r="E14" s="3">
-        <v>24</v>
+      <c r="D14" s="10">
+        <v>17</v>
+      </c>
+      <c r="E14" s="10">
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="3">
+      <c r="A15" s="10">
         <v>13</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="10">
         <v>22.38</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="10">
         <v>51.93</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="10">
         <v>12</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="10">
         <v>12</v>
       </c>
     </row>
@@ -796,19 +1015,19 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A18" s="4">
+      <c r="A18" s="11">
         <v>16</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="11">
         <v>15.99</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="11">
         <v>54</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D18" s="11">
         <v>16</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="11">
         <v>16</v>
       </c>
     </row>
@@ -915,19 +1134,19 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A25" s="4">
+      <c r="A25" s="11">
         <v>23</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B25" s="11">
         <v>22.83</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C25" s="11">
         <v>50.75</v>
       </c>
-      <c r="D25" s="4">
+      <c r="D25" s="11">
         <v>6</v>
       </c>
-      <c r="E25" s="4">
+      <c r="E25" s="11">
         <v>6</v>
       </c>
     </row>
@@ -1000,19 +1219,19 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A30" s="3">
+      <c r="A30" s="10">
         <v>28</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30" s="10">
         <v>22.23</v>
       </c>
-      <c r="C30" s="3">
+      <c r="C30" s="10">
         <v>50.07</v>
       </c>
-      <c r="D30" s="3">
+      <c r="D30" s="10">
         <v>7</v>
       </c>
-      <c r="E30" s="3">
+      <c r="E30" s="10">
         <v>7</v>
       </c>
     </row>
@@ -1196,7 +1415,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView zoomScale="134" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:E12"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1238,10 +1457,10 @@
         <v>52</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
@@ -1423,8 +1642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F23D0A80-5CD4-1941-9FE6-65CA1DE2B111}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1460,10 +1679,10 @@
         <v>52</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
@@ -1646,10 +1865,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1661,115 +1880,371 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="12" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="6" t="s">
+      <c r="B3" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B4" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="6" t="s">
+      <c r="B5" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B6" s="13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="12" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="6" t="s">
+      <c r="B7" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B8" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="12" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="6" t="s">
+      <c r="B9" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B10" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="13" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="6" t="s">
+    <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B13" s="13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="12" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>31</v>
+      <c r="B14" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A40" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A41" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A43" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="B44" s="13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="B45" s="13" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A46" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1797,46 +2272,46 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="G1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="I1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="L1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>28</v>
-      </c>
       <c r="N1" s="5" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>